<commit_message>
Update legend to indicate the gain is for transistor Q4 in schematics
</commit_message>
<xml_diff>
--- a/Data/SmartButton-Battery-Voltage-Divider-Characterization.xlsx
+++ b/Data/SmartButton-Battery-Voltage-Divider-Characterization.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzuni\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GillesZunino-GitHub\SmartButton\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1A9AD3-AF04-445D-922D-AF487E5E9745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C962E8-3708-4A6A-901F-D1AEA514FD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="0" windowWidth="48540" windowHeight="31635" xr2:uid="{139758BB-8A3C-4AD9-B1C0-0F58CC4F6E9C}"/>
   </bookViews>
@@ -149,7 +149,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>h</a:t>
+              <a:t>Q4 - h</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="-25000"/>
@@ -1887,7 +1887,7 @@
   <dimension ref="C7:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>